<commit_message>
Update testcase for Items of DMS_AI
</commit_message>
<xml_diff>
--- a/SRC/Applications/Test.Application/InputTest.xlsx
+++ b/SRC/Applications/Test.Application/InputTest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC18B27-F9D6-4801-8C05-FFB4D0ADE4B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087BFD7C-6B21-4FBD-B806-3B8320CBB090}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="134">
   <si>
     <t>Key</t>
   </si>
@@ -218,6 +218,207 @@
   </si>
   <si>
     <t>.message-content</t>
+  </si>
+  <si>
+    <t>//*[@id='app']/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[1]/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id='app']/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[1]/div/div/div[2]/div[1]/div[1]/ul/li[1]</t>
+  </si>
+  <si>
+    <t>Data.ItemType</t>
+  </si>
+  <si>
+    <t>//*[@id='app']/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[3]/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>Data.UoMInventory</t>
+  </si>
+  <si>
+    <t>//*[@id='app']/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[3]/div/div/div[2]/div[1]/div[1]/ul/li[1]</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.UoMInventory</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[1]/div/div[2]/span[2]/input</t>
+  </si>
+  <si>
+    <t>Xpath.Switchbutton.Active</t>
+  </si>
+  <si>
+    <t>//*[@id="UploadedFile"]</t>
+  </si>
+  <si>
+    <t>Xpath.Avartar</t>
+  </si>
+  <si>
+    <t>D:\anh\avartar.jpg</t>
+  </si>
+  <si>
+    <t>Xpath.Avartar.File</t>
+  </si>
+  <si>
+    <t>Xpath.TextBox.ForeignName</t>
+  </si>
+  <si>
+    <t>Data.ForeignName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên nước ngoài </t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[2]/div[2]/div/input</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[2]/div[1]/div/input</t>
+  </si>
+  <si>
+    <t>Xpath.TextBox.Description</t>
+  </si>
+  <si>
+    <t>Data.Description</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[2]/div[3]/div/input</t>
+  </si>
+  <si>
+    <t>Xpath.TextBox.Barcode</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[2]/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.ItemType</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.UoM</t>
+  </si>
+  <si>
+    <t>Data.UoM</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[2]/div/div/div[2]/div[1]/div[1]/ul/li[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[4]/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.Pricelist</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[4]/div/div/div[2]/div[1]/div[1]/ul/li[2]</t>
+  </si>
+  <si>
+    <t>Data.Pricelist</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[5]/div/input</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.PricingUnit</t>
+  </si>
+  <si>
+    <t>Data.PricingUnit</t>
+  </si>
+  <si>
+    <t>VND</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.UnitPrice</t>
+  </si>
+  <si>
+    <t>Data.UnitPrice</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[3]/div[6]/div/input</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.SaleInfor.UOMCode</t>
+  </si>
+  <si>
+    <t>Data.SaleInfor.UOMCode</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.Purchasinginfor.UOMCode</t>
+  </si>
+  <si>
+    <t>Data.Purchasinginfor.UOMCode</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.SaleInfor.TaxGroup</t>
+  </si>
+  <si>
+    <t>Data.SaleInfor.TaxGroup</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.Purchasinginfor.TaxGroup</t>
+  </si>
+  <si>
+    <t>DataPurchasinginfor.TaxGroup</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[4]/div[1]/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[4]/div[1]/div/div/div[2]/div[1]/div[1]/ul/li[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[4]/div[2]/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[4]/div[2]/div/div/div[2]/div[1]/div[1]/ul/li[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[5]/div[1]/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[5]/div[1]/div/div/div[2]/div[1]/div[1]/ul/li[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[5]/div[2]/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[1]/div[5]/div[2]/div/div/div[2]/div[1]/div[1]/ul/li[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/ul/li[2]/span</t>
+  </si>
+  <si>
+    <t>Xpath.Tab.Itemgroup</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[2]/div[1]/div/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[2]/div[1]/div/div/div/div[2]/div[1]/div[1]/ul/li[1]</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.Itemgroup</t>
+  </si>
+  <si>
+    <t>Data.Itemgroup</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[2]/div[2]/div[1]/div/div/div[1]/input</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div/div/div/div[2]/form/div[2]/div[2]/div[2]/div[1]/div/div/div[2]/div[1]/div[1]/ul/li[1]</t>
+  </si>
+  <si>
+    <t>Xpath.Dropdown.Attribute1</t>
+  </si>
+  <si>
+    <t>Data.Attribute1</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/main/div/div/div[3]/div[1]/div/input</t>
+  </si>
+  <si>
+    <t>Xpath.List.Search</t>
   </si>
 </sst>
 </file>
@@ -627,13 +828,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,7 +842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -649,7 +850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -657,7 +858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -665,7 +866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -692,16 +893,16 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
-    <col min="7" max="7" width="24.88671875" customWidth="1"/>
+    <col min="1" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -724,7 +925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -747,7 +948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -770,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -801,21 +1002,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" customWidth="1"/>
-    <col min="4" max="4" width="110.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" customWidth="1"/>
+    <col min="4" max="4" width="110.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -829,7 +1030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -843,7 +1044,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -857,7 +1058,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -871,7 +1072,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -885,7 +1086,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -899,7 +1100,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -913,7 +1114,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -927,7 +1128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -941,7 +1142,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -955,7 +1156,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -969,7 +1170,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -983,7 +1184,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -997,7 +1198,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1011,7 +1212,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1019,94 +1220,570 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
         <v>55</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
         <v>59</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
+        <v>127</v>
+      </c>
+      <c r="D49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="D50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" t="s">
         <v>63</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D52" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
         <v>65</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D54" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1791,7 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="D8" r:id="rId2" xr:uid="{F37103F0-02CF-4E2E-8D6F-18A52338B1F3}"/>
-    <hyperlink ref="D20" r:id="rId3" xr:uid="{EEE100E2-6F9B-40C8-BAD8-011A6445DBE0}"/>
+    <hyperlink ref="D53" r:id="rId3" xr:uid="{EEE100E2-6F9B-40C8-BAD8-011A6445DBE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>